<commit_message>
Update SRS & Req Coverage & Add the Design Document
Co-Authored-By: hyhdsj <118108177+hyhdsj@users.noreply.github.com>
Co-Authored-By: MENG-GUANLIN(Green) <88531334+paopaolin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Documents/COMP3211 Project G13 PIM Requirements Coverage Report.xlsx
+++ b/Documents/COMP3211 Project G13 PIM Requirements Coverage Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgl/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidjiang/Desktop/GitHub Repo/personal-information-manager/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88C37B1-8F92-C545-A26A-2EC85B075E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7A1C49-1E48-2441-8F05-C1B9D5DAB249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16440" xr2:uid="{A13E7134-B716-814C-8B61-8A4A9B515359}"/>
+    <workbookView xWindow="4360" yWindow="760" windowWidth="30200" windowHeight="19980" xr2:uid="{A13E7134-B716-814C-8B61-8A4A9B515359}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>User Story</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,10 +129,6 @@
   </si>
   <si>
     <t>NFR04</t>
-  </si>
-  <si>
-    <t>NFR06</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -148,7 +144,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -162,30 +158,68 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>✔</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>︎</t>
+    </r>
+  </si>
+  <si>
+    <t>NFR06</t>
+  </si>
+  <si>
+    <t>NFR07</t>
+  </si>
+  <si>
     <t>✕</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>tips:all the USR&amp;SFR/NFR details could be checked in SRS document</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR08</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>NFR09</t>
+  </si>
+  <si>
+    <t>NFR05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -205,6 +239,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Segoe UI Symbol"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Segoe UI Symbol"/>
       <family val="2"/>
     </font>
@@ -231,7 +279,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -241,9 +289,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -259,7 +313,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -555,13 +609,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDDCB56-EC34-F742-9333-F14303E6EBC4}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
@@ -569,7 +623,7 @@
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,203 +637,235 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24">
+    <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="18">
-      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="C16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18">
+      <c r="D16" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
         <v>33</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>